<commit_message>
Update followers and posts data
</commit_message>
<xml_diff>
--- a/bsky_followers.xlsx
+++ b/bsky_followers.xlsx
@@ -1,110 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samue\bsky-tracker\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{865B3C55-8B85-4C11-83E7-C29D37B3E49A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>nea-ukcharity.bsky.social</t>
-  </si>
-  <si>
-    <t>caneurope.bsky.social</t>
-  </si>
-  <si>
-    <t>wateraid.bsky.social</t>
-  </si>
-  <si>
-    <t>migrantsrights.bsky.social</t>
-  </si>
-  <si>
-    <t>friends-earth.bsky.social</t>
-  </si>
-  <si>
-    <t>samcardwell44.bsky.social</t>
-  </si>
-  <si>
-    <t>greenpeace.eu</t>
-  </si>
-  <si>
-    <t>wwfeu.bsky.social</t>
-  </si>
-  <si>
-    <t>powertochange.org.uk</t>
-  </si>
-  <si>
-    <t>thegreenregister.bsky.social</t>
-  </si>
-  <si>
-    <t>endfuelpoverty.bsky.social</t>
-  </si>
-  <si>
-    <t>commenergyengland.bsky.social</t>
-  </si>
-  <si>
-    <t>extinctionrebellion.uk</t>
-  </si>
-  <si>
-    <t>wwtworldwide.bsky.social</t>
-  </si>
-  <si>
-    <t>bristolgreenparty.bsky.social</t>
-  </si>
-  <si>
-    <t>warmthiswinter.bsky.social</t>
-  </si>
-  <si>
-    <t>jrct.bsky.social</t>
-  </si>
-  <si>
-    <t>ssencommunity.bsky.social</t>
-  </si>
-  <si>
-    <t>localtrust.bsky.social</t>
-  </si>
-  <si>
-    <t>wiltscouncil.bsky.social</t>
-  </si>
-  <si>
-    <t>nationalgrid.bsky.social</t>
-  </si>
-  <si>
-    <t>ofgem.bsky.social</t>
-  </si>
-  <si>
-    <t>barnsleycouncil.bsky.social</t>
-  </si>
-  <si>
-    <t>northsomersetc.bsky.social</t>
-  </si>
-  <si>
-    <t>citizensadvice.bsky.social</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,21 +63,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -204,7 +107,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -238,7 +141,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -273,10 +175,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -449,93 +350,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:Z2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>date</t>
+        </is>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>25</v>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2025-01-21</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>